<commit_message>
Added PDF Export for User Report.
</commit_message>
<xml_diff>
--- a/src/SFA/wwwroot/resources/reports/Users.xlsx
+++ b/src/SFA/wwwroot/resources/reports/Users.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>User Id</t>
   </si>
@@ -140,7 +140,7 @@
     <t>(641) 660-4654</t>
   </si>
   <si>
-    <t>3</t>
+    <t>1</t>
   </si>
   <si>
     <t>Jonny Mukherjee</t>
@@ -296,9 +296,6 @@
     <t>testMission@gmail.com</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>TroyTest Reynolds</t>
   </si>
   <si>
@@ -309,6 +306,18 @@
   </si>
   <si>
     <t>Florida Section 4</t>
+  </si>
+  <si>
+    <t>TroyTest3 Reynolds</t>
+  </si>
+  <si>
+    <t>troytreynolds2@gmail.com</t>
+  </si>
+  <si>
+    <t>troytreynolds4@gmail.com</t>
+  </si>
+  <si>
+    <t>troytreynolds5@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -366,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -987,7 +996,7 @@
         <v>35</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29">
@@ -995,23 +1004,80 @@
         <v>55</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <v>58</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>98</v>
       </c>
+      <c r="C30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="3">
+        <v>60</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="3">
+        <v>59</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
   </sheetData>
   <headerFooter/>

</xml_diff>